<commit_message>
normalised mark prediction dataset excel file in added
</commit_message>
<xml_diff>
--- a/gradient_Descent/student-mat1.xlsx
+++ b/gradient_Descent/student-mat1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsme\Downloads\project\gradient_Descent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsme\Downloads\project\prediction_model\gradient_Descent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1005A416-0D2E-445B-A339-80689FEF5E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5703B8-708D-47BC-9B3E-1CD2E0AE3F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="student-mat" sheetId="1" r:id="rId1"/>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>